<commit_message>
Second motor works. ADD changes to timer choice in stepper_init
</commit_message>
<xml_diff>
--- a/Kinematics_Prototype/SOFT/Ports_STM32G431.xlsx
+++ b/Kinematics_Prototype/SOFT/Ports_STM32G431.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Documents\GitRepos\Modular_3D_Printer\Kinematics_Prototype\SOFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BEFB37-1FBF-4CD7-BE76-448AED4D938E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D7F600-704F-4691-B56E-5D5DEDFDB275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BC4E02F5-8D92-42C1-A265-7B617E91710A}"/>
   </bookViews>
@@ -298,7 +298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="194">
   <si>
     <t>Pin</t>
   </si>
@@ -1097,13 +1097,16 @@
 GPIO</t>
   </si>
   <si>
-    <t>PUL+ STEP0</t>
-  </si>
-  <si>
     <t>DIR- STEP1</t>
   </si>
   <si>
     <t>PULL- STEP1</t>
+  </si>
+  <si>
+    <t>PULL- STEP2</t>
+  </si>
+  <si>
+    <t>DIR- STEP2</t>
   </si>
 </sst>
 </file>
@@ -2429,10 +2432,10 @@
   <dimension ref="B1:AM35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,7 +2570,7 @@
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F5" s="74" t="s">
         <v>181</v>
@@ -2619,7 +2622,7 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F6" s="75" t="s">
         <v>182</v>
@@ -2728,7 +2731,9 @@
         <v>13</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="F9" s="76" t="s">
         <v>183</v>
       </c>
@@ -2776,7 +2781,9 @@
         <v>17</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="F10" s="76" t="s">
         <v>184</v>
       </c>
@@ -3115,7 +3122,9 @@
         <v>22</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="F18" s="78" t="s">
         <v>188</v>
       </c>
@@ -3150,10 +3159,10 @@
       <c r="C19" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E19" s="2"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="F19" s="76" t="s">
         <v>189</v>
       </c>

</xml_diff>

<commit_message>
Most stuff works, just need to fix UART commands
</commit_message>
<xml_diff>
--- a/Kinematics_Prototype/SOFT/Ports_STM32G431.xlsx
+++ b/Kinematics_Prototype/SOFT/Ports_STM32G431.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Documents\GitRepos\Modular_3D_Printer\Kinematics_Prototype\SOFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59091FA3-3CD6-4F87-A670-DED49D56C0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A6975E-775C-4DE3-97E3-9536AF4655F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BC4E02F5-8D92-42C1-A265-7B617E91710A}"/>
   </bookViews>
@@ -298,7 +298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="194">
   <si>
     <t>Pin</t>
   </si>
@@ -1103,7 +1103,10 @@
     <t>PULL- STEP1</t>
   </si>
   <si>
-    <t>STEP2</t>
+    <t>DIR- STEP2</t>
+  </si>
+  <si>
+    <t>PULL- STEP2</t>
   </si>
 </sst>
 </file>
@@ -2432,7 +2435,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2729,7 +2732,7 @@
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F9" s="76" t="s">
         <v>183</v>

</xml_diff>

<commit_message>
New version with interupt timer...
</commit_message>
<xml_diff>
--- a/Kinematics_Prototype/SOFT/Ports_STM32G431.xlsx
+++ b/Kinematics_Prototype/SOFT/Ports_STM32G431.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Documents\GitRepos\Modular_3D_Printer\Kinematics_Prototype\SOFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8140D5BF-3036-43CE-8264-4A88A2466714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A68151-CCFB-431F-9FC9-90AA801523FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BC4E02F5-8D92-42C1-A265-7B617E91710A}"/>
   </bookViews>
@@ -2432,10 +2432,10 @@
   <dimension ref="B1:AM35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2731,9 +2731,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="2" t="s">
-        <v>192</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="76" t="s">
         <v>183</v>
       </c>
@@ -2923,7 +2921,9 @@
         <v>19</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="F13" s="76" t="s">
         <v>187</v>
       </c>

</xml_diff>